<commit_message>
features added, ready to deploy
added welcome funciton, can take file path and has the option to save to folder

will print successfully created message at the end
</commit_message>
<xml_diff>
--- a/Copy of invoice  packing list 217-22486085 112件 一主11分.xlsx
+++ b/Copy of invoice  packing list 217-22486085 112件 一主11分.xlsx
@@ -21,6 +21,12 @@
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'12件ZENGTUO'!$A$11:$M$24</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'2件CAISHENG'!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>

</xml_diff>

<commit_message>
created a GUI version
</commit_message>
<xml_diff>
--- a/Copy of invoice  packing list 217-22486085 112件 一主11分.xlsx
+++ b/Copy of invoice  packing list 217-22486085 112件 一主11分.xlsx
@@ -21,6 +21,34 @@
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'12件ZENGTUO'!$A$11:$M$24</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'2件CAISHENG'!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">2件CAISHENG!$A$11:$P$23</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">12件ZENGTUO!$A$11:$M$24</definedName>

</xml_diff>